<commit_message>
web version and APP
</commit_message>
<xml_diff>
--- a/tavriav.ua.xlsx
+++ b/tavriav.ua.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="201">
   <si>
     <t>QA engineer:</t>
   </si>
@@ -667,18 +667,7 @@
     <t>Order is successfully created with unique ID. Notification was sent on your e-mail.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>Browsers:</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> 
-Chrome  84.0.4147.105
-Opera 69.0.3686.77
-Firefox 79.0</t>
-    </r>
+    <t>Таврия В - APP on Google</t>
   </si>
   <si>
     <r>
@@ -688,7 +677,7 @@
       <t>OS</t>
     </r>
     <r>
-      <t>: Windows 10 Pro</t>
+      <t>: Android 9.1</t>
     </r>
   </si>
   <si>
@@ -717,44 +706,158 @@
       <rPr>
         <b/>
       </rPr>
-      <t>Open browser</t>
-    </r>
-    <r>
-      <t xml:space="preserve">
+      <t xml:space="preserve">Open APP Таврия В
+version 2.3.2
 </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">Clear browser cookies and cache
-Open </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <color rgb="FF1155CC"/>
-        <u/>
-      </rPr>
-      <t>https://tavriav.ua/</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <t>ver. 1.02</t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Block #1: Download from stores                        </t>
+  </si>
+  <si>
+    <t>Actual result:</t>
+  </si>
+  <si>
+    <t>1. Search APP "Таврия В" on Google Play</t>
+  </si>
+  <si>
+    <t>APP is finded and can be download.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block #2: Main page/account                        </t>
+  </si>
+  <si>
+    <t>1. Tap "Account" to the left top side of screen.</t>
+  </si>
+  <si>
+    <t>Registration and Sign in buttons are visible.</t>
+  </si>
+  <si>
+    <t>2. Tap on "Registration" button</t>
+  </si>
+  <si>
+    <t>Registration page is opened.</t>
+  </si>
+  <si>
+    <t>3. Tap on "Sign in" button</t>
+  </si>
+  <si>
+    <t>Authoriztion page is opened.</t>
+  </si>
+  <si>
+    <t>4. Tap on "Forgot password"</t>
+  </si>
+  <si>
+    <t>Forgot password form is opened.</t>
+  </si>
+  <si>
+    <t>5. Tap on "Settings" inside your account</t>
+  </si>
+  <si>
+    <t>Settings is opened.</t>
+  </si>
+  <si>
+    <t>6. Select your defualt city from list</t>
+  </si>
+  <si>
+    <t>List with cities is shown.</t>
+  </si>
+  <si>
+    <t>7. Tap "My orders" inside account</t>
+  </si>
+  <si>
+    <t>Your previous orders is shown.</t>
+  </si>
+  <si>
+    <t>8. Tap on barcode scanner to the right top side of screen</t>
+  </si>
+  <si>
+    <t>Barcode scanner is opened.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Tap on QR-code </t>
+  </si>
+  <si>
+    <t>Popup window with unique QR-code with your bonus points is shown</t>
+  </si>
+  <si>
+    <t>10. Tap on your account name</t>
+  </si>
+  <si>
+    <t>Personal page with preferences is opened.</t>
+  </si>
+  <si>
+    <t>11. Tap "Share with friends"</t>
+  </si>
+  <si>
+    <t>Popup window with different sending methods is opened.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block #3: Search                    </t>
+  </si>
+  <si>
+    <t>2. Tap on any item from the list</t>
+  </si>
+  <si>
+    <t>3. Enter any valid goods name to the search field (only numbers)</t>
+  </si>
+  <si>
+    <t>4. Enter any special symbols to the search field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block #4: Shop/Catalog                    </t>
+  </si>
+  <si>
+    <t>1. Tap and open on catalog in any category</t>
+  </si>
+  <si>
+    <t>Goods is added to the cart. Count of added goods displayed on the cart.</t>
+  </si>
+  <si>
+    <t>3. Increase counts of added goods, tap '+'</t>
+  </si>
+  <si>
+    <t>4. Decrease counts of added goods, tap '-'</t>
+  </si>
+  <si>
+    <t>5. Tap on the small picture from the left side in any goods category.</t>
+  </si>
+  <si>
+    <t>6. Tap on the 'Filter' on the left top side of screen and choose that what you need, 'Brand' for example.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block #5: Checkout                    </t>
+  </si>
+  <si>
+    <t>1. Add goods what you need to the cart. Tap on the cart-icon to the right top side of screen</t>
+  </si>
+  <si>
+    <t>Checkout (cart) page is opened.</t>
+  </si>
+  <si>
+    <t>2. Change count of any goods in the cart, tap '+' or '-'</t>
+  </si>
+  <si>
+    <t>3. Delete any goods from the cart, tap on 'delete' icon</t>
+  </si>
+  <si>
+    <t>"Confirm" popup window is shown. Choosed goods is deleted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Press 'Submit order' </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order is successfully created with unique ID. </t>
+  </si>
+  <si>
+    <t>No connection with database.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -849,6 +952,12 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="36.0"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1002,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1138,6 +1247,31 @@
     </xf>
     <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3027,80 +3161,484 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="57.57"/>
-    <col customWidth="1" min="7" max="7" width="56.29"/>
+    <col customWidth="1" min="2" max="2" width="51.71"/>
+    <col customWidth="1" min="3" max="3" width="49.14"/>
+    <col customWidth="1" min="4" max="4" width="26.86"/>
+    <col customWidth="1" min="5" max="5" width="67.14"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
+      <c r="C2" s="52" t="s">
+        <v>150</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="G3" s="7"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4">
       <c r="B4" s="8"/>
       <c r="C4" s="6"/>
-      <c r="G4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="6"/>
-      <c r="G5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6">
       <c r="B6" s="10" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C6" s="6"/>
-      <c r="G6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7">
-      <c r="B7" s="10" t="s">
-        <v>151</v>
+      <c r="B7" s="11" t="s">
+        <v>152</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="G7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8">
-      <c r="B8" s="11" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="12" t="s">
+      <c r="B8" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="54" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="14">
+      <c r="B14" s="54" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17">
+      <c r="B17" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="28"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="28"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="28"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D20" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="28"/>
+    </row>
+    <row r="21">
+      <c r="B21" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="28"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="41" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="28"/>
+    </row>
+    <row r="23">
+      <c r="B23" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="28"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="28"/>
+    </row>
+    <row r="25">
+      <c r="B25" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="28"/>
+    </row>
+    <row r="26">
+      <c r="B26" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="C26" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="D26" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="28"/>
+    </row>
+    <row r="28">
+      <c r="B28" s="54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="28"/>
+    </row>
+    <row r="31">
+      <c r="B31" s="46" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="28"/>
+    </row>
+    <row r="32">
+      <c r="B32" s="43" t="s">
+        <v>183</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="28"/>
+    </row>
+    <row r="33">
+      <c r="B33" s="24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="28"/>
+    </row>
+    <row r="35">
+      <c r="B35" s="54" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="D37" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="58"/>
+    </row>
+    <row r="38">
+      <c r="B38" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>187</v>
+      </c>
+      <c r="D38" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="58"/>
+    </row>
+    <row r="39">
+      <c r="B39" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="28"/>
+    </row>
+    <row r="40">
+      <c r="B40" s="49" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="28"/>
+    </row>
+    <row r="41">
+      <c r="B41" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="C41" s="59" t="s">
+        <v>113</v>
+      </c>
+      <c r="D41" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="28"/>
+    </row>
+    <row r="42">
+      <c r="B42" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="C42" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="28"/>
+    </row>
+    <row r="44">
+      <c r="B44" s="54" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="43" t="s">
+        <v>193</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>194</v>
+      </c>
+      <c r="D46" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E46" s="28"/>
+    </row>
+    <row r="47">
+      <c r="B47" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E47" s="28"/>
+    </row>
+    <row r="48">
+      <c r="B48" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>197</v>
+      </c>
+      <c r="D48" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49">
+      <c r="B49" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="D49" s="60" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="51" t="s">
+        <v>200</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:G9"/>
+  <mergeCells count="6">
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="C2:E8"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B44:E44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
-    <hyperlink r:id="rId2" ref="B9"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>